<commit_message>
Actualisation de la liste excel
</commit_message>
<xml_diff>
--- a/ListeTransaction.xlsx
+++ b/ListeTransaction.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\SourceTree\OS-TP3-99\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22110" windowHeight="9555"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="22116" windowHeight="9552"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>NoTransaction</t>
   </si>
@@ -29,18 +24,6 @@
     <t>Données</t>
   </si>
   <si>
-    <t>Nom utilisateur et mot de passe</t>
-  </si>
-  <si>
-    <t>Confirmation de l'identification</t>
-  </si>
-  <si>
-    <t>Envoie d'une carte à un joueur</t>
-  </si>
-  <si>
-    <t>Choix d'une carte par un joueur</t>
-  </si>
-  <si>
     <t>Partie terminée</t>
   </si>
   <si>
@@ -68,12 +51,6 @@
     <t>08;</t>
   </si>
   <si>
-    <t>Erreur lors de l'identification</t>
-  </si>
-  <si>
-    <t>03;1;2</t>
-  </si>
-  <si>
     <t>02;</t>
   </si>
   <si>
@@ -83,7 +60,31 @@
     <t>06;player1;999;player2;99;…;player10;1</t>
   </si>
   <si>
-    <t>04;1;2;99</t>
+    <t>Connexion</t>
+  </si>
+  <si>
+    <t>Connexion réussie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erreur lors de l'autentification </t>
+  </si>
+  <si>
+    <t>Carte piochée</t>
+  </si>
+  <si>
+    <t>Carte choisie</t>
+  </si>
+  <si>
+    <t>Carte jouée</t>
+  </si>
+  <si>
+    <t>03;objet carte</t>
+  </si>
+  <si>
+    <t>To DO</t>
+  </si>
+  <si>
+    <t>04;objet carte; nom du joueur; nouveau total</t>
   </si>
 </sst>
 </file>
@@ -140,8 +141,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:C10" totalsRowShown="0">
-  <autoFilter ref="A1:C10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:C11" totalsRowShown="0">
+  <autoFilter ref="A1:C11"/>
   <tableColumns count="3">
     <tableColumn id="1" name="NoTransaction"/>
     <tableColumn id="2" name="Données"/>
@@ -194,7 +195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,7 +230,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -438,20 +439,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
-    <col min="3" max="4" width="44.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="3" max="4" width="44.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,106 +460,117 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -576,7 +588,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -588,7 +600,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualisation du fichier excel
</commit_message>
<xml_diff>
--- a/ListeTransaction.xlsx
+++ b/ListeTransaction.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\GitHub\OS-TP3-99\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="48" windowWidth="22116" windowHeight="9552"/>
   </bookViews>
@@ -81,10 +86,10 @@
     <t>03;objet carte</t>
   </si>
   <si>
-    <t>To DO</t>
-  </si>
-  <si>
     <t>04;objet carte; nom du joueur; nouveau total</t>
+  </si>
+  <si>
+    <t>05;objet carte</t>
   </si>
 </sst>
 </file>
@@ -195,7 +200,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,7 +235,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -442,7 +447,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -474,7 +479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -507,7 +512,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -515,7 +520,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -526,7 +531,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>